<commit_message>
Tables edited in Chapter 2
</commit_message>
<xml_diff>
--- a/text/analysis.xlsx
+++ b/text/analysis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>GIS software</t>
   </si>
@@ -867,6 +867,143 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Infobars</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - general information and warnings for all users</t>
+    </r>
+  </si>
+  <si>
+    <t>GRASS GIS before GSoC</t>
+  </si>
+  <si>
+    <t>GRASS GIS after GSoC</t>
+  </si>
+  <si>
+    <t>same as before GSoC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Yes, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>it is displayed almost always. It is not displayed only if we use the --text Flag, or if we specify by argument the mapset we want to open.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>No features</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <t>Features enhancing first-time user experience</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Warehouse (.mdb)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - has the character of a location. You need to define it first, then connect to it. It has a clearly defined coordinate system. One GeoWorkspace file can have multiple Warehouses attached.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Project file (.qvsproj)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- as GRASS workspace (.gxw)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Project</t>
     </r>
     <r>
@@ -878,7 +1015,128 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - similar to GRASS database</t>
+      <t xml:space="preserve"> contains layers</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file (.sprj)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - as GRASS workspace (.gxw)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Project file (.qgz) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- as GRASS workspace (.gxw)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file (.aprx)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - similar to GRASS workspace (.gxw)</t>
     </r>
   </si>
   <si>
@@ -903,219 +1161,55 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - as GRASS database</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Warehouse </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(.mdb) - has the character of a location. You need to define it first, then connect to it. It has a clearly defined coordinate system. One GeoWorkspace file can have multiple Warehouses attached.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Workspace</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - as GRASS database</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Project </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- as GRASS database or location, project contains layers, similar to QGIS 3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Infobars</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - general information and warnings for all users</t>
-    </r>
-  </si>
-  <si>
-    <t>GRASS GIS before GSoC</t>
-  </si>
-  <si>
-    <t>GRASS GIS after GSoC</t>
-  </si>
-  <si>
-    <t>same as before GSoC</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Yes, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>it is displayed almost always. It is not displayed only if we use the --text Flag, or if we specify by argument the mapset we want to open.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>No features</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-  </si>
-  <si>
-    <t>Features enhancing first-time user experience</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Project</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - as GRASS database or location, project contains layers</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Project</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - as GRASS database, is created only when we save the settings to a SAGA GIS project file.</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file (.gws)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- as GRASS workspace (.gxw)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Workspace file (.wor)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - as GRASS workspace (.gxw)</t>
     </r>
   </si>
 </sst>
@@ -1543,7 +1637,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1596,101 +1690,104 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1975,8 +2072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1995,36 +2092,36 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:4" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>61</v>
+      <c r="D2" s="20" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="1:4" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="33" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2036,7 +2133,7 @@
       <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="39"/>
+      <c r="D5" s="31"/>
     </row>
     <row r="6" spans="1:4" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="37"/>
@@ -2051,89 +2148,89 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="40" t="s">
+      <c r="B7" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="41" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="46"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="42"/>
     </row>
     <row r="9" spans="1:4" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="46"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="42"/>
     </row>
     <row r="10" spans="1:4" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="21" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="46"/>
+      <c r="D10" s="42"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="46" t="s">
+      <c r="A11" s="22"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="42" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="46"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="42"/>
     </row>
     <row r="13" spans="1:4" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="33" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="46"/>
+      <c r="D13" s="42"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="47" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="43" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="47"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="43"/>
     </row>
     <row r="16" spans="1:4" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="29"/>
-      <c r="B16" s="44"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="26"/>
-      <c r="D16" s="48"/>
+      <c r="D16" s="44"/>
     </row>
     <row r="17" spans="1:4" ht="57.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="21" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>20</v>
@@ -2143,11 +2240,11 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="25" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="13" t="s">
@@ -2155,7 +2252,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="29"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="7" t="s">
         <v>24</v>
       </c>
@@ -2171,51 +2268,53 @@
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="24" t="s">
-        <v>61</v>
+      <c r="D21" s="20" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="51" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
     </row>
     <row r="23" spans="1:4" ht="24.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="34" t="s">
-        <v>62</v>
+      <c r="B23" s="52" t="s">
+        <v>61</v>
       </c>
       <c r="C23" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="51" t="s">
+      <c r="D23" s="45" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="41"/>
+      <c r="B24" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="28"/>
     </row>
     <row r="25" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="21"/>
+      <c r="C25" s="25"/>
       <c r="D25" s="15" t="s">
         <v>29</v>
       </c>
@@ -2225,94 +2324,94 @@
       <c r="B26" s="26"/>
       <c r="C26" s="26"/>
       <c r="D26" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="43.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="38" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="24" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
-      <c r="B28" s="21" t="s">
+      <c r="A28" s="39"/>
+      <c r="B28" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
     </row>
     <row r="29" spans="1:4" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="50"/>
+      <c r="A29" s="39"/>
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
     </row>
     <row r="30" spans="1:4" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="47" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="31"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="48"/>
     </row>
     <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="B32" s="21" t="s">
+      <c r="A32" s="48"/>
+      <c r="B32" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="31"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="48"/>
     </row>
     <row r="33" spans="1:5" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="31"/>
-      <c r="B33" s="21"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="25"/>
       <c r="C33" s="26"/>
-      <c r="D33" s="32"/>
+      <c r="D33" s="49"/>
     </row>
     <row r="34" spans="1:5" ht="51.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="47" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="50" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="31"/>
+      <c r="A35" s="48"/>
       <c r="B35" s="18" t="s">
         <v>48</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="23"/>
+      <c r="D35" s="51"/>
     </row>
     <row r="36" spans="1:5" ht="409.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19"/>
@@ -2321,49 +2420,49 @@
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:5" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="24" t="s">
-        <v>61</v>
+      <c r="D37" s="20" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
+      <c r="A38" s="46"/>
+      <c r="B38" s="46"/>
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
     </row>
     <row r="39" spans="1:5" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
-        <v>56</v>
+      <c r="A39" s="21" t="s">
+        <v>51</v>
       </c>
       <c r="B39" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>60</v>
+      <c r="C39" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="24" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
+      <c r="A40" s="22"/>
       <c r="B40" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
     </row>
     <row r="41" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="29"/>
+      <c r="A41" s="23"/>
       <c r="B41" s="9" t="s">
         <v>44</v>
       </c>
@@ -2372,30 +2471,30 @@
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B42" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="20" t="s">
+      <c r="A42" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D42" s="24" t="s">
         <v>49</v>
       </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="28"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="1"/>
@@ -2443,31 +2542,23 @@
       <c r="E50" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B9:B16"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B2:B3"/>
+  <mergeCells count="47">
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A16"/>
     <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B2:B3"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="C23:C26"/>
@@ -2477,6 +2568,18 @@
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="D14:D16"/>
     <mergeCell ref="D23:D24"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B9:B16"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A27:A29"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="A39:A41"/>
     <mergeCell ref="A37:A38"/>
@@ -2487,11 +2590,6 @@
     <mergeCell ref="C39:C41"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
   </mergeCells>
   <pageMargins left="0.11811023622047245" right="3.937007874015748E-2" top="7.874015748031496E-2" bottom="7.874015748031496E-2" header="0.11811023622047245" footer="0.11811023622047245"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>